<commit_message>
EPBDS: added collection item discriminator feature.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/hints/FieldHintsSupportTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/hints/FieldHintsSupportTest.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>classA</t>
   </si>
@@ -104,9 +103,6 @@
     <t>org.openl.rules.mapping.to</t>
   </si>
   <si>
-    <t>ChildA,A</t>
-  </si>
-  <si>
     <t>fieldAType</t>
   </si>
   <si>
@@ -119,19 +115,10 @@
     <t>ChildA</t>
   </si>
   <si>
-    <t>oneWay</t>
-  </si>
-  <si>
-    <t>ChildA,ChildA</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
     <t>ChildA, A</t>
-  </si>
-  <si>
-    <t>//Data Mapping mappings2</t>
   </si>
   <si>
     <t>array[6]</t>
@@ -191,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -218,17 +205,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -284,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -293,16 +269,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -311,25 +285,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +597,7 @@
   <dimension ref="C4:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -666,13 +636,13 @@
     <row r="7" spans="3:11">
       <c r="C7" s="8"/>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="3:11">
       <c r="C8" s="8"/>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="3:11">
@@ -709,10 +679,10 @@
         <v>13</v>
       </c>
       <c r="J13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="3:11">
@@ -736,10 +706,10 @@
         <v>13</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="3:11">
@@ -755,8 +725,8 @@
       <c r="F15" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="3:11">
       <c r="C16" t="s">
@@ -771,10 +741,10 @@
       <c r="F16" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="3:11">
       <c r="C17" t="s">
@@ -789,10 +759,10 @@
       <c r="F17" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="14"/>
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="3:11">
       <c r="C18" t="s">
@@ -808,7 +778,7 @@
         <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -827,28 +797,28 @@
       <c r="F19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16" t="s">
+      <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="14"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="3:11">
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="14"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="3:11">
       <c r="C21" t="s">
@@ -861,12 +831,12 @@
         <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="3:11">
       <c r="C22" t="s">
@@ -879,24 +849,18 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="14"/>
+        <v>36</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="4"/>
       <c r="K22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:C8"/>
@@ -910,163 +874,14 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C7:L11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="7" spans="3:12">
-      <c r="C7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="3:12">
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12">
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12">
-      <c r="C10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12">
-      <c r="C11" s="14"/>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="F10:F11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>